<commit_message>
TRUNG FIX CHỜ MINH HIẾU
</commit_message>
<xml_diff>
--- a/Sprint 2/Tài liệu đặc tả yêu cầu/Kiểm thử ONLY QUẠT PART 2.xlsx
+++ b/Sprint 2/Tài liệu đặc tả yêu cầu/Kiểm thử ONLY QUẠT PART 2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Acer\Documents\GitHub\BCS\Sprint 2\Tài liệu đặc tả yêu cầu\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CC677B8-9267-485C-AE25-775B42382CE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90353523-F217-4838-9006-EEE06E0F1E5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{C21961AB-009A-468A-8C50-42DFE010BB31}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="143">
   <si>
     <t>Test case: Trang tìm kiếm BCS</t>
   </si>
@@ -246,15 +246,6 @@
     <t>Đánh giá</t>
   </si>
   <si>
-    <t>Đánh giá bằng 1 số bất kỳ</t>
-  </si>
-  <si>
-    <t>1.Nhấn vào ô đánh giá
-2.Nhập số
-3.Nhấn [Đánh giá]
-4.F5</t>
-  </si>
-  <si>
     <t>Phải hiển thị tên cùng giá trị đánh giá đã nhập</t>
   </si>
   <si>
@@ -279,18 +270,6 @@
     <t>Đã đưa chỉ số đánh giá về 0</t>
   </si>
   <si>
-    <t>Đánh giá bằng chữ và số</t>
-  </si>
-  <si>
-    <t>1.Nhấn vào ô đánh giá
-2.Nhập chữ và số
-3.Nhấn [Đánh giá]
-4.F5</t>
-  </si>
-  <si>
-    <t>1a,2b,3c</t>
-  </si>
-  <si>
     <t>Tìm kiếm</t>
   </si>
   <si>
@@ -325,9 +304,6 @@
     <t>E_2</t>
   </si>
   <si>
-    <t>E_3</t>
-  </si>
-  <si>
     <t>E_4</t>
   </si>
   <si>
@@ -347,12 +323,6 @@
   </si>
   <si>
     <t>Trạng thái</t>
-  </si>
-  <si>
-    <t>5,1</t>
-  </si>
-  <si>
-    <t>Chưa đưa chỉ số đánh giá về 0</t>
   </si>
   <si>
     <t>Test case: Trang trò chuyện BCS</t>
@@ -533,6 +503,18 @@
   </si>
   <si>
     <t>Hiển thị đánh giá bao gồm tên đăng nhập và số sao</t>
+  </si>
+  <si>
+    <t>1.Nhấn vào ô đánh giá
+2.Vote số sao
+3.Nhấn [Đánh giá]
+4.F5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vote </t>
+  </si>
+  <si>
+    <t>Đánh giá bằng số sao vote bất kỳ</t>
   </si>
 </sst>
 </file>
@@ -1246,7 +1228,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7054C498-8387-4232-8AE0-A330C02A2385}">
   <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
@@ -1521,10 +1503,10 @@
         <v>31</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="F14" s="11" t="s">
         <v>47</v>
@@ -1545,7 +1527,7 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="29" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="B17" s="29"/>
       <c r="C17" s="29"/>
@@ -1608,13 +1590,13 @@
         <v>33</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="D20" s="12" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="F20" s="11" t="s">
         <v>47</v>
@@ -1635,13 +1617,13 @@
       </c>
       <c r="B21" s="26"/>
       <c r="C21" s="11" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="D21" s="12" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="E21" s="10" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="F21" s="11" t="s">
         <v>47</v>
@@ -1808,7 +1790,7 @@
         <v>57</v>
       </c>
       <c r="E30" s="10" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="F30" s="11" t="s">
         <v>47</v>
@@ -1825,17 +1807,17 @@
     </row>
     <row r="31" spans="1:9" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="9" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="B31" s="26"/>
       <c r="C31" s="8" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="D31" s="15" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="E31" s="10" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="F31" s="11" t="s">
         <v>47</v>
@@ -1852,17 +1834,17 @@
     </row>
     <row r="32" spans="1:9" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="9" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="B32" s="26"/>
       <c r="C32" s="8" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="D32" s="15" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="E32" s="10" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="F32" s="11" t="s">
         <v>47</v>
@@ -1879,14 +1861,14 @@
     </row>
     <row r="33" spans="1:9" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="9" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="B33" s="26"/>
       <c r="C33" s="8" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="D33" s="15" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="E33" s="10" t="s">
         <v>58</v>
@@ -1929,10 +1911,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68FE9BBC-A729-407C-A7F1-8BCC2741D4DA}">
-  <dimension ref="A1:J28"/>
+  <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1983,22 +1965,22 @@
         <v>3</v>
       </c>
       <c r="C3" s="20" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D3" s="21" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="E3" s="21" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="F3" s="20" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="G3" s="20" t="s">
         <v>6</v>
       </c>
       <c r="H3" s="20" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="I3" s="22" t="s">
         <v>61</v>
@@ -2009,25 +1991,25 @@
     </row>
     <row r="4" spans="1:10" ht="70.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="17" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="B4" s="31" t="s">
         <v>63</v>
       </c>
       <c r="C4" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="E4" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="F4" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="D4" s="17" t="s">
+      <c r="G4" s="17" t="s">
         <v>65</v>
-      </c>
-      <c r="E4" s="17" t="s">
-        <v>94</v>
-      </c>
-      <c r="F4" s="17" t="s">
-        <v>66</v>
-      </c>
-      <c r="G4" s="17" t="s">
-        <v>67</v>
       </c>
       <c r="H4" s="17" t="s">
         <v>40</v>
@@ -2037,23 +2019,23 @@
     </row>
     <row r="5" spans="1:10" ht="71.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="17" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="B5" s="32"/>
       <c r="C5" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="D5" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="E5" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="D5" s="17" t="s">
+      <c r="F5" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="G5" s="17" t="s">
         <v>70</v>
-      </c>
-      <c r="F5" s="17" t="s">
-        <v>71</v>
-      </c>
-      <c r="G5" s="17" t="s">
-        <v>72</v>
       </c>
       <c r="H5" s="17" t="s">
         <v>40</v>
@@ -2061,100 +2043,101 @@
       <c r="I5" s="18"/>
       <c r="J5" s="18"/>
     </row>
-    <row r="6" spans="1:10" ht="74.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="17" t="s">
+    <row r="6" spans="1:10" ht="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="7" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="8" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="34" t="s">
+        <v>105</v>
+      </c>
+      <c r="B8" s="35"/>
+      <c r="C8" s="36"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="17"/>
+      <c r="I8" s="18"/>
+      <c r="J8" s="18"/>
+    </row>
+    <row r="9" spans="1:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="37" t="s">
+        <v>60</v>
+      </c>
+      <c r="B9" s="38"/>
+      <c r="C9" s="38"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
+      <c r="G9" s="38"/>
+      <c r="H9" s="38"/>
+      <c r="I9" s="38"/>
+      <c r="J9" s="39"/>
+    </row>
+    <row r="10" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="D10" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="E10" s="21" t="s">
+        <v>85</v>
+      </c>
+      <c r="F10" s="20" t="s">
         <v>86</v>
       </c>
-      <c r="B6" s="33"/>
-      <c r="C6" s="17" t="s">
+      <c r="G10" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="H10" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="I10" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="J10" s="23" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="B11" s="31" t="s">
+        <v>71</v>
+      </c>
+      <c r="C11" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="D11" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="D6" s="17" t="s">
+      <c r="E11" s="17" t="s">
         <v>74</v>
       </c>
-      <c r="E6" s="17" t="s">
+      <c r="F11" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="F6" s="17" t="s">
-        <v>71</v>
-      </c>
-      <c r="G6" s="17" t="s">
-        <v>95</v>
-      </c>
-      <c r="H6" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="I6" s="18"/>
-      <c r="J6" s="18"/>
-    </row>
-    <row r="8" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="9" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="34" t="s">
-        <v>113</v>
-      </c>
-      <c r="B9" s="35"/>
-      <c r="C9" s="36"/>
-      <c r="D9" s="17"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="17"/>
-      <c r="G9" s="17"/>
-      <c r="H9" s="17"/>
-      <c r="I9" s="18"/>
-      <c r="J9" s="18"/>
-    </row>
-    <row r="10" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="37" t="s">
-        <v>60</v>
-      </c>
-      <c r="B10" s="38"/>
-      <c r="C10" s="38"/>
-      <c r="D10" s="38"/>
-      <c r="E10" s="38"/>
-      <c r="F10" s="38"/>
-      <c r="G10" s="38"/>
-      <c r="H10" s="38"/>
-      <c r="I10" s="38"/>
-      <c r="J10" s="39"/>
-    </row>
-    <row r="11" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="B11" s="20" t="s">
-        <v>3</v>
-      </c>
-      <c r="C11" s="20" t="s">
-        <v>89</v>
-      </c>
-      <c r="D11" s="21" t="s">
-        <v>90</v>
-      </c>
-      <c r="E11" s="21" t="s">
-        <v>91</v>
-      </c>
-      <c r="F11" s="20" t="s">
-        <v>92</v>
-      </c>
-      <c r="G11" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="H11" s="20" t="s">
-        <v>93</v>
-      </c>
-      <c r="I11" s="22" t="s">
-        <v>61</v>
-      </c>
-      <c r="J11" s="23" t="s">
-        <v>62</v>
-      </c>
+      <c r="G11" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="H11" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="I11" s="18"/>
+      <c r="J11" s="18"/>
     </row>
     <row r="12" spans="1:10" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="17" t="s">
-        <v>87</v>
-      </c>
-      <c r="B12" s="31" t="s">
-        <v>76</v>
-      </c>
+        <v>82</v>
+      </c>
+      <c r="B12" s="33"/>
       <c r="C12" s="17" t="s">
         <v>77</v>
       </c>
@@ -2162,13 +2145,13 @@
         <v>78</v>
       </c>
       <c r="E12" s="17" t="s">
-        <v>79</v>
+        <v>17</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="G12" s="17" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="H12" s="17" t="s">
         <v>40</v>
@@ -2176,114 +2159,114 @@
       <c r="I12" s="18"/>
       <c r="J12" s="18"/>
     </row>
-    <row r="13" spans="1:10" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="17" t="s">
-        <v>88</v>
-      </c>
-      <c r="B13" s="33"/>
-      <c r="C13" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="D13" s="17" t="s">
+    <row r="13" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="14" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="34" t="s">
+        <v>106</v>
+      </c>
+      <c r="B14" s="35"/>
+      <c r="C14" s="36"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="17"/>
+      <c r="H14" s="17"/>
+      <c r="I14" s="18"/>
+      <c r="J14" s="18"/>
+    </row>
+    <row r="15" spans="1:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="37" t="s">
+        <v>60</v>
+      </c>
+      <c r="B15" s="38"/>
+      <c r="C15" s="38"/>
+      <c r="D15" s="38"/>
+      <c r="E15" s="38"/>
+      <c r="F15" s="38"/>
+      <c r="G15" s="38"/>
+      <c r="H15" s="38"/>
+      <c r="I15" s="38"/>
+      <c r="J15" s="39"/>
+    </row>
+    <row r="16" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="B16" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" s="20" t="s">
         <v>83</v>
       </c>
-      <c r="E13" s="17" t="s">
+      <c r="D16" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="E16" s="21" t="s">
+        <v>85</v>
+      </c>
+      <c r="F16" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="G16" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="H16" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="I16" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="J16" s="23" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="24" t="s">
+        <v>109</v>
+      </c>
+      <c r="B17" s="31" t="s">
+        <v>116</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="D17" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="E17" s="24" t="s">
+        <v>112</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="G17" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="H17" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="I17" s="18"/>
+      <c r="J17" s="18"/>
+    </row>
+    <row r="18" spans="1:10" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="B18" s="33"/>
+      <c r="C18" s="17" t="s">
+        <v>115</v>
+      </c>
+      <c r="D18" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="E18" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="F13" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="G13" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="H13" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="I13" s="18"/>
-      <c r="J13" s="18"/>
-    </row>
-    <row r="14" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="15" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="34" t="s">
-        <v>114</v>
-      </c>
-      <c r="B15" s="35"/>
-      <c r="C15" s="36"/>
-      <c r="D15" s="17"/>
-      <c r="E15" s="17"/>
-      <c r="F15" s="17"/>
-      <c r="G15" s="17"/>
-      <c r="H15" s="17"/>
-      <c r="I15" s="18"/>
-      <c r="J15" s="18"/>
-    </row>
-    <row r="16" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="37" t="s">
-        <v>60</v>
-      </c>
-      <c r="B16" s="38"/>
-      <c r="C16" s="38"/>
-      <c r="D16" s="38"/>
-      <c r="E16" s="38"/>
-      <c r="F16" s="38"/>
-      <c r="G16" s="38"/>
-      <c r="H16" s="38"/>
-      <c r="I16" s="38"/>
-      <c r="J16" s="39"/>
-    </row>
-    <row r="17" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="B17" s="20" t="s">
-        <v>3</v>
-      </c>
-      <c r="C17" s="20" t="s">
-        <v>89</v>
-      </c>
-      <c r="D17" s="21" t="s">
-        <v>90</v>
-      </c>
-      <c r="E17" s="21" t="s">
-        <v>91</v>
-      </c>
-      <c r="F17" s="20" t="s">
-        <v>92</v>
-      </c>
-      <c r="G17" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="H17" s="20" t="s">
-        <v>93</v>
-      </c>
-      <c r="I17" s="22" t="s">
-        <v>61</v>
-      </c>
-      <c r="J17" s="23" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="24" t="s">
-        <v>117</v>
-      </c>
-      <c r="B18" s="31" t="s">
-        <v>124</v>
-      </c>
-      <c r="C18" s="12" t="s">
-        <v>118</v>
-      </c>
-      <c r="D18" s="17" t="s">
-        <v>119</v>
-      </c>
-      <c r="E18" s="24" t="s">
-        <v>120</v>
-      </c>
-      <c r="F18" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="G18" s="8" t="s">
-        <v>121</v>
+      <c r="F18" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="G18" s="17" t="s">
+        <v>76</v>
       </c>
       <c r="H18" s="17" t="s">
         <v>40</v>
@@ -2291,114 +2274,114 @@
       <c r="I18" s="18"/>
       <c r="J18" s="18"/>
     </row>
-    <row r="19" spans="1:10" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="17" t="s">
+    <row r="20" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="21" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="34" t="s">
+        <v>117</v>
+      </c>
+      <c r="B21" s="35"/>
+      <c r="C21" s="36"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="17"/>
+      <c r="F21" s="17"/>
+      <c r="G21" s="17"/>
+      <c r="H21" s="17"/>
+      <c r="I21" s="18"/>
+      <c r="J21" s="18"/>
+    </row>
+    <row r="22" spans="1:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="37" t="s">
+        <v>60</v>
+      </c>
+      <c r="B22" s="38"/>
+      <c r="C22" s="38"/>
+      <c r="D22" s="38"/>
+      <c r="E22" s="38"/>
+      <c r="F22" s="38"/>
+      <c r="G22" s="38"/>
+      <c r="H22" s="38"/>
+      <c r="I22" s="38"/>
+      <c r="J22" s="39"/>
+    </row>
+    <row r="23" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="B23" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="C23" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="D23" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="E23" s="21" t="s">
+        <v>85</v>
+      </c>
+      <c r="F23" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="G23" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="H23" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="I23" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="J23" s="23" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="24" t="s">
+        <v>123</v>
+      </c>
+      <c r="B24" s="31" t="s">
+        <v>118</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="D24" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="E24" s="25" t="s">
+        <v>121</v>
+      </c>
+      <c r="F24" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="B19" s="33"/>
-      <c r="C19" s="17" t="s">
-        <v>123</v>
-      </c>
-      <c r="D19" s="17" t="s">
-        <v>83</v>
-      </c>
-      <c r="E19" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="F19" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="G19" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="H19" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="I19" s="18"/>
-      <c r="J19" s="18"/>
-    </row>
-    <row r="21" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="22" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="34" t="s">
+      <c r="G24" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="H24" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="I24" s="18"/>
+      <c r="J24" s="18"/>
+    </row>
+    <row r="25" spans="1:10" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="17" t="s">
+        <v>124</v>
+      </c>
+      <c r="B25" s="32"/>
+      <c r="C25" s="17" t="s">
         <v>125</v>
       </c>
-      <c r="B22" s="35"/>
-      <c r="C22" s="36"/>
-      <c r="D22" s="17"/>
-      <c r="E22" s="17"/>
-      <c r="F22" s="17"/>
-      <c r="G22" s="17"/>
-      <c r="H22" s="17"/>
-      <c r="I22" s="18"/>
-      <c r="J22" s="18"/>
-    </row>
-    <row r="23" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="37" t="s">
-        <v>60</v>
-      </c>
-      <c r="B23" s="38"/>
-      <c r="C23" s="38"/>
-      <c r="D23" s="38"/>
-      <c r="E23" s="38"/>
-      <c r="F23" s="38"/>
-      <c r="G23" s="38"/>
-      <c r="H23" s="38"/>
-      <c r="I23" s="38"/>
-      <c r="J23" s="39"/>
-    </row>
-    <row r="24" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="B24" s="20" t="s">
-        <v>3</v>
-      </c>
-      <c r="C24" s="20" t="s">
-        <v>89</v>
-      </c>
-      <c r="D24" s="21" t="s">
-        <v>90</v>
-      </c>
-      <c r="E24" s="21" t="s">
-        <v>91</v>
-      </c>
-      <c r="F24" s="20" t="s">
-        <v>92</v>
-      </c>
-      <c r="G24" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="H24" s="20" t="s">
-        <v>93</v>
-      </c>
-      <c r="I24" s="22" t="s">
-        <v>61</v>
-      </c>
-      <c r="J24" s="23" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="24" t="s">
+      <c r="D25" s="17" t="s">
+        <v>126</v>
+      </c>
+      <c r="E25" s="17" t="s">
         <v>131</v>
       </c>
-      <c r="B25" s="31" t="s">
-        <v>126</v>
-      </c>
-      <c r="C25" s="12" t="s">
+      <c r="F25" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="D25" s="17" t="s">
-        <v>128</v>
-      </c>
-      <c r="E25" s="25" t="s">
-        <v>129</v>
-      </c>
-      <c r="F25" s="8" t="s">
-        <v>130</v>
-      </c>
-      <c r="G25" s="8" t="s">
-        <v>130</v>
+      <c r="G25" s="5" t="s">
+        <v>127</v>
       </c>
       <c r="H25" s="17" t="s">
         <v>40</v>
@@ -2406,25 +2389,25 @@
       <c r="I25" s="18"/>
       <c r="J25" s="18"/>
     </row>
-    <row r="26" spans="1:10" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:10" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="17" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B26" s="32"/>
       <c r="C26" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="D26" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="E26" s="17" t="s">
+        <v>132</v>
+      </c>
+      <c r="F26" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="D26" s="17" t="s">
-        <v>134</v>
-      </c>
-      <c r="E26" s="17" t="s">
-        <v>139</v>
-      </c>
-      <c r="F26" s="5" t="s">
-        <v>135</v>
-      </c>
       <c r="G26" s="5" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="H26" s="17" t="s">
         <v>40</v>
@@ -2432,25 +2415,25 @@
       <c r="I26" s="18"/>
       <c r="J26" s="18"/>
     </row>
-    <row r="27" spans="1:10" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:10" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="17" t="s">
+        <v>124</v>
+      </c>
+      <c r="B27" s="33"/>
+      <c r="C27" s="17" t="s">
+        <v>134</v>
+      </c>
+      <c r="D27" s="17" t="s">
+        <v>135</v>
+      </c>
+      <c r="E27" s="17" t="s">
         <v>136</v>
       </c>
-      <c r="B27" s="32"/>
-      <c r="C27" s="17" t="s">
+      <c r="F27" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="D27" s="17" t="s">
-        <v>138</v>
-      </c>
-      <c r="E27" s="17" t="s">
-        <v>140</v>
-      </c>
-      <c r="F27" s="5" t="s">
-        <v>141</v>
-      </c>
       <c r="G27" s="5" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="H27" s="17" t="s">
         <v>40</v>
@@ -2458,46 +2441,20 @@
       <c r="I27" s="18"/>
       <c r="J27" s="18"/>
     </row>
-    <row r="28" spans="1:10" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="17" t="s">
-        <v>132</v>
-      </c>
-      <c r="B28" s="33"/>
-      <c r="C28" s="17" t="s">
-        <v>142</v>
-      </c>
-      <c r="D28" s="17" t="s">
-        <v>143</v>
-      </c>
-      <c r="E28" s="17" t="s">
-        <v>144</v>
-      </c>
-      <c r="F28" s="5" t="s">
-        <v>145</v>
-      </c>
-      <c r="G28" s="5" t="s">
-        <v>145</v>
-      </c>
-      <c r="H28" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="I28" s="18"/>
-      <c r="J28" s="18"/>
-    </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="B25:B28"/>
-    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="B24:B27"/>
+    <mergeCell ref="B17:B18"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A2:J2"/>
-    <mergeCell ref="B4:B6"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="A10:J10"/>
-    <mergeCell ref="A23:J23"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="A15:C15"/>
-    <mergeCell ref="A16:J16"/>
-    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="A9:J9"/>
+    <mergeCell ref="A22:J22"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="A15:J15"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="B4:B5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
MHIEUU đã sửa xong
</commit_message>
<xml_diff>
--- a/Sprint 2/Tài liệu đặc tả yêu cầu/Kiểm thử ONLY QUẠT PART 2.xlsx
+++ b/Sprint 2/Tài liệu đặc tả yêu cầu/Kiểm thử ONLY QUẠT PART 2.xlsx
@@ -5,39 +5,28 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Acer\Documents\GitHub\BCS\Sprint 2\Tài liệu đặc tả yêu cầu\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://wru-my.sharepoint.com/personal/2251061780_e_tlu_edu_vn/Documents/Tài liệu/GitHub/BCS/Sprint 2/Tài liệu đặc tả yêu cầu/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90353523-F217-4838-9006-EEE06E0F1E5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{90353523-F217-4838-9006-EEE06E0F1E5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{24FAE130-EB3D-4F3B-B5F4-2F547348D5BF}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{C21961AB-009A-468A-8C50-42DFE010BB31}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="1" xr2:uid="{C21961AB-009A-468A-8C50-42DFE010BB31}"/>
   </bookViews>
   <sheets>
     <sheet name="Giao diện" sheetId="1" r:id="rId1"/>
     <sheet name="Bên Trong" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="144">
   <si>
     <t>Test case: Trang tìm kiếm BCS</t>
   </si>
@@ -264,26 +253,9 @@
     <t>abc, xyz</t>
   </si>
   <si>
-    <t>Phải đưa chỉ số đánh giá về 0</t>
-  </si>
-  <si>
-    <t>Đã đưa chỉ số đánh giá về 0</t>
-  </si>
-  <si>
     <t>Tìm kiếm</t>
   </si>
   <si>
-    <t>Tìm kiếm bằng 1 ký tự bất kỳ</t>
-  </si>
-  <si>
-    <t>1.Nhấn vào ô tìm kiếm
-2.Nhập ký tự
-3.Bấm [tìm kiếm]</t>
-  </si>
-  <si>
-    <t>h,a,b</t>
-  </si>
-  <si>
     <t>Phải chạy tìm kiếm</t>
   </si>
   <si>
@@ -291,11 +263,6 @@
   </si>
   <si>
     <t>Không nhập gì vào ô tìm kiếm</t>
-  </si>
-  <si>
-    <t>1.Nhấn vào ô tìm kiếm
-2.Không nhập ký tự
-3.Bấm [tìm kiếm]</t>
   </si>
   <si>
     <t>E_1</t>
@@ -406,11 +373,6 @@
     <t>Trò chuyện với chủ cho thuê</t>
   </si>
   <si>
-    <t xml:space="preserve">1.Nhấn bài viết
-2.Chọn [Liên hệ]
-</t>
-  </si>
-  <si>
     <t>Chat box</t>
   </si>
   <si>
@@ -418,9 +380,6 @@
   </si>
   <si>
     <t>E_7</t>
-  </si>
-  <si>
-    <t>Không cho phép lời nói xúc phạm</t>
   </si>
   <si>
     <t>Trò chuyện</t>
@@ -514,7 +473,41 @@
     <t xml:space="preserve">Vote </t>
   </si>
   <si>
-    <t>Đánh giá bằng số sao vote bất kỳ</t>
+    <t>Đánh giá bằng số sao vote từ 1 đến 5</t>
+  </si>
+  <si>
+    <t>Tìm kiếm bằng bộ lọc</t>
+  </si>
+  <si>
+    <t>1.Chọn Thuê trọ
+2.Chọn các đặc điểm về phòng trọ 
+3.Bấm [Lọc]</t>
+  </si>
+  <si>
+    <t>Chọn đặc điểm trên thanh bộ lọc</t>
+  </si>
+  <si>
+    <t>Hiển thị các phòng trọ có đặc điểm giống với phòng đã chọn</t>
+  </si>
+  <si>
+    <t>1.Chọn Thuê trọ
+2.Không nhập ký tự
+3.Bấm [Lọc]</t>
+  </si>
+  <si>
+    <t>Trò chuyện với admin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.Nhấn bài viết
+2.Chọn [Liên hệ]    3.Nhập chữ hoặc số vào khung chat
+</t>
+  </si>
+  <si>
+    <t>1.Chọn [Chat với admin]
+2.Nhập chữ hoặc số vào khung chat</t>
+  </si>
+  <si>
+    <t>Hiện thị tên cùng đánh giá đã nhập</t>
   </si>
 </sst>
 </file>
@@ -1232,16 +1225,16 @@
       <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="2" max="2" width="11.33203125" customWidth="1"/>
-    <col min="3" max="3" width="15.5546875" customWidth="1"/>
-    <col min="4" max="4" width="34.21875" customWidth="1"/>
-    <col min="5" max="5" width="27.109375" customWidth="1"/>
-    <col min="6" max="6" width="15.21875" customWidth="1"/>
+    <col min="3" max="3" width="15.53125" customWidth="1"/>
+    <col min="4" max="4" width="34.19921875" customWidth="1"/>
+    <col min="5" max="5" width="27.1328125" customWidth="1"/>
+    <col min="6" max="6" width="15.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
@@ -1256,7 +1249,7 @@
       <c r="H1" s="28"/>
       <c r="I1" s="28"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A2" s="27" t="s">
         <v>1</v>
       </c>
@@ -1269,7 +1262,7 @@
       <c r="H2" s="27"/>
       <c r="I2" s="27"/>
     </row>
-    <row r="3" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1298,7 +1291,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="78.599999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" ht="78.599999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A4" s="9" t="s">
         <v>8</v>
       </c>
@@ -1327,7 +1320,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A5" s="9" t="s">
         <v>13</v>
       </c>
@@ -1354,7 +1347,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="53.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" ht="53.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A6" s="9" t="s">
         <v>18</v>
       </c>
@@ -1381,7 +1374,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="48.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" ht="48.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A7" s="9" t="s">
         <v>21</v>
       </c>
@@ -1408,7 +1401,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A10" s="29" t="s">
         <v>24</v>
       </c>
@@ -1423,7 +1416,7 @@
       <c r="H10" s="28"/>
       <c r="I10" s="28"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A11" s="27" t="s">
         <v>1</v>
       </c>
@@ -1436,7 +1429,7 @@
       <c r="H11" s="27"/>
       <c r="I11" s="27"/>
     </row>
-    <row r="12" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A12" s="1" t="s">
         <v>2</v>
       </c>
@@ -1465,7 +1458,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" ht="28.9" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A13" s="9" t="s">
         <v>25</v>
       </c>
@@ -1494,7 +1487,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" ht="57.4" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A14" s="9" t="s">
         <v>30</v>
       </c>
@@ -1503,10 +1496,10 @@
         <v>31</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="F14" s="11" t="s">
         <v>47</v>
@@ -1521,13 +1514,13 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
       <c r="B15" s="7"/>
       <c r="F15" s="11"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A17" s="29" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="B17" s="29"/>
       <c r="C17" s="29"/>
@@ -1540,7 +1533,7 @@
       <c r="H17" s="28"/>
       <c r="I17" s="28"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A18" s="27" t="s">
         <v>1</v>
       </c>
@@ -1553,7 +1546,7 @@
       <c r="H18" s="27"/>
       <c r="I18" s="27"/>
     </row>
-    <row r="19" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A19" s="1" t="s">
         <v>2</v>
       </c>
@@ -1582,7 +1575,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" ht="57.4" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A20" s="9" t="s">
         <v>32</v>
       </c>
@@ -1590,13 +1583,13 @@
         <v>33</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="D20" s="12" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="F20" s="11" t="s">
         <v>47</v>
@@ -1611,19 +1604,19 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" ht="57.4" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A21" s="9" t="s">
         <v>34</v>
       </c>
       <c r="B21" s="26"/>
       <c r="C21" s="11" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D21" s="12" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="E21" s="10" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="F21" s="11" t="s">
         <v>47</v>
@@ -1638,7 +1631,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A24" s="29" t="s">
         <v>41</v>
       </c>
@@ -1653,7 +1646,7 @@
       <c r="H24" s="28"/>
       <c r="I24" s="28"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A25" s="27" t="s">
         <v>1</v>
       </c>
@@ -1666,7 +1659,7 @@
       <c r="H25" s="27"/>
       <c r="I25" s="27"/>
     </row>
-    <row r="26" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A26" s="1" t="s">
         <v>2</v>
       </c>
@@ -1695,7 +1688,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:9" ht="43.15" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A27" s="9" t="s">
         <v>42</v>
       </c>
@@ -1724,7 +1717,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:9" ht="57.4" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A28" s="9" t="s">
         <v>48</v>
       </c>
@@ -1751,7 +1744,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="71.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:9" ht="71.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A29" s="9" t="s">
         <v>51</v>
       </c>
@@ -1778,7 +1771,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:9" ht="57.4" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A30" s="9" t="s">
         <v>55</v>
       </c>
@@ -1790,7 +1783,7 @@
         <v>57</v>
       </c>
       <c r="E30" s="10" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="F30" s="11" t="s">
         <v>47</v>
@@ -1805,19 +1798,19 @@
         <v>39</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:9" ht="43.15" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A31" s="9" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="B31" s="26"/>
       <c r="C31" s="8" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="D31" s="15" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="E31" s="10" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="F31" s="11" t="s">
         <v>47</v>
@@ -1832,19 +1825,19 @@
         <v>40</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:9" ht="57.4" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A32" s="9" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="B32" s="26"/>
       <c r="C32" s="8" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="D32" s="15" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="E32" s="10" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="F32" s="11" t="s">
         <v>47</v>
@@ -1859,16 +1852,16 @@
         <v>40</v>
       </c>
     </row>
-    <row r="33" spans="1:9" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:9" ht="43.15" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A33" s="9" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="B33" s="26"/>
       <c r="C33" s="8" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="D33" s="15" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="E33" s="10" t="s">
         <v>58</v>
@@ -1913,23 +1906,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68FE9BBC-A729-407C-A7F1-8BCC2741D4DA}">
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="12.6640625" customWidth="1"/>
-    <col min="2" max="2" width="14.5546875" customWidth="1"/>
+    <col min="2" max="2" width="14.53125" customWidth="1"/>
     <col min="3" max="3" width="12" customWidth="1"/>
-    <col min="4" max="4" width="20.21875" customWidth="1"/>
-    <col min="5" max="5" width="15.88671875" customWidth="1"/>
-    <col min="6" max="6" width="22.5546875" customWidth="1"/>
-    <col min="7" max="7" width="23.44140625" customWidth="1"/>
+    <col min="4" max="4" width="20.19921875" customWidth="1"/>
+    <col min="5" max="5" width="15.86328125" customWidth="1"/>
+    <col min="6" max="6" width="22.53125" customWidth="1"/>
+    <col min="7" max="7" width="23.46484375" customWidth="1"/>
     <col min="8" max="8" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A1" s="34" t="s">
         <v>59</v>
       </c>
@@ -1943,7 +1936,7 @@
       <c r="I1" s="18"/>
       <c r="J1" s="18"/>
     </row>
-    <row r="2" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A2" s="37" t="s">
         <v>60</v>
       </c>
@@ -1957,7 +1950,7 @@
       <c r="I2" s="38"/>
       <c r="J2" s="39"/>
     </row>
-    <row r="3" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A3" s="19" t="s">
         <v>2</v>
       </c>
@@ -1965,22 +1958,22 @@
         <v>3</v>
       </c>
       <c r="C3" s="20" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="D3" s="21" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="E3" s="21" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="F3" s="20" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="G3" s="20" t="s">
         <v>6</v>
       </c>
       <c r="H3" s="20" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="I3" s="22" t="s">
         <v>61</v>
@@ -1989,21 +1982,21 @@
         <v>62</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="70.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" ht="70.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A4" s="17" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B4" s="31" t="s">
         <v>63</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="D4" s="17" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="E4" s="17" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="F4" s="17" t="s">
         <v>64</v>
@@ -2017,9 +2010,9 @@
       <c r="I4" s="18"/>
       <c r="J4" s="18"/>
     </row>
-    <row r="5" spans="1:10" ht="71.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" ht="71.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A5" s="17" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="B5" s="32"/>
       <c r="C5" s="17" t="s">
@@ -2032,10 +2025,10 @@
         <v>68</v>
       </c>
       <c r="F5" s="17" t="s">
-        <v>69</v>
+        <v>143</v>
       </c>
       <c r="G5" s="17" t="s">
-        <v>70</v>
+        <v>143</v>
       </c>
       <c r="H5" s="17" t="s">
         <v>40</v>
@@ -2043,11 +2036,11 @@
       <c r="I5" s="18"/>
       <c r="J5" s="18"/>
     </row>
-    <row r="6" spans="1:10" ht="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="7" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="8" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" ht="16.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="7" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="8" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A8" s="34" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="B8" s="35"/>
       <c r="C8" s="36"/>
@@ -2059,7 +2052,7 @@
       <c r="I8" s="18"/>
       <c r="J8" s="18"/>
     </row>
-    <row r="9" spans="1:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A9" s="37" t="s">
         <v>60</v>
       </c>
@@ -2073,7 +2066,7 @@
       <c r="I9" s="38"/>
       <c r="J9" s="39"/>
     </row>
-    <row r="10" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A10" s="19" t="s">
         <v>2</v>
       </c>
@@ -2081,22 +2074,22 @@
         <v>3</v>
       </c>
       <c r="C10" s="20" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="D10" s="21" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="E10" s="21" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="F10" s="20" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="G10" s="20" t="s">
         <v>6</v>
       </c>
       <c r="H10" s="20" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="I10" s="22" t="s">
         <v>61</v>
@@ -2105,27 +2098,27 @@
         <v>62</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" ht="57.4" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A11" s="17" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="B11" s="31" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C11" s="17" t="s">
-        <v>72</v>
+        <v>135</v>
       </c>
       <c r="D11" s="17" t="s">
-        <v>73</v>
+        <v>136</v>
       </c>
       <c r="E11" s="17" t="s">
-        <v>74</v>
+        <v>137</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>75</v>
+        <v>138</v>
       </c>
       <c r="G11" s="17" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="H11" s="17" t="s">
         <v>40</v>
@@ -2133,25 +2126,25 @@
       <c r="I11" s="18"/>
       <c r="J11" s="18"/>
     </row>
-    <row r="12" spans="1:10" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" ht="43.15" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A12" s="17" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="B12" s="33"/>
       <c r="C12" s="17" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D12" s="17" t="s">
-        <v>78</v>
+        <v>139</v>
       </c>
       <c r="E12" s="17" t="s">
         <v>17</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="G12" s="17" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="H12" s="17" t="s">
         <v>40</v>
@@ -2159,10 +2152,10 @@
       <c r="I12" s="18"/>
       <c r="J12" s="18"/>
     </row>
-    <row r="13" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="14" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="14" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A14" s="34" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="B14" s="35"/>
       <c r="C14" s="36"/>
@@ -2174,7 +2167,7 @@
       <c r="I14" s="18"/>
       <c r="J14" s="18"/>
     </row>
-    <row r="15" spans="1:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A15" s="37" t="s">
         <v>60</v>
       </c>
@@ -2188,7 +2181,7 @@
       <c r="I15" s="38"/>
       <c r="J15" s="39"/>
     </row>
-    <row r="16" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A16" s="19" t="s">
         <v>2</v>
       </c>
@@ -2196,22 +2189,22 @@
         <v>3</v>
       </c>
       <c r="C16" s="20" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="D16" s="21" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="E16" s="21" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="F16" s="20" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="G16" s="20" t="s">
         <v>6</v>
       </c>
       <c r="H16" s="20" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="I16" s="22" t="s">
         <v>61</v>
@@ -2220,27 +2213,27 @@
         <v>62</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" ht="71.650000000000006" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A17" s="24" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="B17" s="31" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="D17" s="17" t="s">
-        <v>111</v>
+        <v>141</v>
       </c>
       <c r="E17" s="24" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="G17" s="8" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="H17" s="17" t="s">
         <v>40</v>
@@ -2248,25 +2241,25 @@
       <c r="I17" s="18"/>
       <c r="J17" s="18"/>
     </row>
-    <row r="18" spans="1:10" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" ht="43.15" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A18" s="17" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="B18" s="33"/>
       <c r="C18" s="17" t="s">
-        <v>115</v>
+        <v>140</v>
       </c>
       <c r="D18" s="17" t="s">
-        <v>78</v>
+        <v>142</v>
       </c>
       <c r="E18" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="F18" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="G18" s="17" t="s">
-        <v>76</v>
+        <v>105</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="G18" s="8" t="s">
+        <v>106</v>
       </c>
       <c r="H18" s="17" t="s">
         <v>40</v>
@@ -2274,10 +2267,10 @@
       <c r="I18" s="18"/>
       <c r="J18" s="18"/>
     </row>
-    <row r="20" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="21" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="21" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A21" s="34" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="B21" s="35"/>
       <c r="C21" s="36"/>
@@ -2289,7 +2282,7 @@
       <c r="I21" s="18"/>
       <c r="J21" s="18"/>
     </row>
-    <row r="22" spans="1:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A22" s="37" t="s">
         <v>60</v>
       </c>
@@ -2303,7 +2296,7 @@
       <c r="I22" s="38"/>
       <c r="J22" s="39"/>
     </row>
-    <row r="23" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A23" s="19" t="s">
         <v>2</v>
       </c>
@@ -2311,22 +2304,22 @@
         <v>3</v>
       </c>
       <c r="C23" s="20" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="D23" s="21" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="E23" s="21" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="F23" s="20" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="G23" s="20" t="s">
         <v>6</v>
       </c>
       <c r="H23" s="20" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="I23" s="22" t="s">
         <v>61</v>
@@ -2335,27 +2328,27 @@
         <v>62</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:10" ht="57.4" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A24" s="24" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="B24" s="31" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="D24" s="17" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="E24" s="25" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="F24" s="8" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="G24" s="8" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="H24" s="17" t="s">
         <v>40</v>
@@ -2363,25 +2356,25 @@
       <c r="I24" s="18"/>
       <c r="J24" s="18"/>
     </row>
-    <row r="25" spans="1:10" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:10" ht="57.4" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A25" s="17" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="B25" s="32"/>
       <c r="C25" s="17" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="D25" s="17" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="E25" s="17" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="H25" s="17" t="s">
         <v>40</v>
@@ -2389,25 +2382,25 @@
       <c r="I25" s="18"/>
       <c r="J25" s="18"/>
     </row>
-    <row r="26" spans="1:10" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:10" ht="43.15" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A26" s="17" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B26" s="32"/>
       <c r="C26" s="17" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="D26" s="17" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="E26" s="17" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="G26" s="5" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="H26" s="17" t="s">
         <v>40</v>
@@ -2415,25 +2408,25 @@
       <c r="I26" s="18"/>
       <c r="J26" s="18"/>
     </row>
-    <row r="27" spans="1:10" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:10" ht="28.9" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A27" s="17" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="B27" s="33"/>
       <c r="C27" s="17" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="D27" s="17" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="E27" s="17" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="H27" s="17" t="s">
         <v>40</v>

</xml_diff>

<commit_message>
Trung fix phần đánh giá
</commit_message>
<xml_diff>
--- a/Sprint 2/Tài liệu đặc tả yêu cầu/Kiểm thử ONLY QUẠT PART 2.xlsx
+++ b/Sprint 2/Tài liệu đặc tả yêu cầu/Kiểm thử ONLY QUẠT PART 2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Acer\Documents\GitHub\BCS\Sprint 2\Tài liệu đặc tả yêu cầu\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2776037-5D78-4803-B960-9195437E8723}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{885CEB03-2C4F-40E0-9E2D-FA9AECC5263A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{C21961AB-009A-468A-8C50-42DFE010BB31}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{C21961AB-009A-468A-8C50-42DFE010BB31}"/>
   </bookViews>
   <sheets>
     <sheet name="Giao diện" sheetId="1" r:id="rId1"/>
@@ -1224,7 +1224,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7054C498-8387-4232-8AE0-A330C02A2385}">
   <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
@@ -1909,8 +1909,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68FE9BBC-A729-407C-A7F1-8BCC2741D4DA}">
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2034,7 +2034,7 @@
         <v>143</v>
       </c>
       <c r="H5" s="17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I5" s="18"/>
       <c r="J5" s="18"/>

</xml_diff>

<commit_message>
MHIEU nhờ Trung sửa
</commit_message>
<xml_diff>
--- a/Sprint 2/Tài liệu đặc tả yêu cầu/Kiểm thử ONLY QUẠT PART 2.xlsx
+++ b/Sprint 2/Tài liệu đặc tả yêu cầu/Kiểm thử ONLY QUẠT PART 2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\OneDrive - Thuyloi University\Tài liệu\GitHub\BCS\Sprint 2\Tài liệu đặc tả yêu cầu\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Acer\Documents\GitHub\BCS\Sprint 2\Tài liệu đặc tả yêu cầu\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F759633-7769-458D-B2AB-5699C4F63EB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{671256D1-55DC-4DE3-B9A5-E171AC26DD9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="1" xr2:uid="{C21961AB-009A-468A-8C50-42DFE010BB31}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{C21961AB-009A-468A-8C50-42DFE010BB31}"/>
   </bookViews>
   <sheets>
     <sheet name="Giao diện" sheetId="1" r:id="rId1"/>
@@ -83,9 +83,6 @@
     <t>Hiển thị toàn bộ trọ gần đây được đăng</t>
   </si>
   <si>
-    <t>NULL</t>
-  </si>
-  <si>
     <t>D_22</t>
   </si>
   <si>
@@ -259,12 +256,6 @@
     <t>Phải chạy tìm kiếm</t>
   </si>
   <si>
-    <t>Chạy tìm kiếm</t>
-  </si>
-  <si>
-    <t>Không nhập gì vào ô tìm kiếm</t>
-  </si>
-  <si>
     <t>E_1</t>
   </si>
   <si>
@@ -490,11 +481,6 @@
     <t>Hiển thị các phòng trọ có đặc điểm giống với phòng đã chọn</t>
   </si>
   <si>
-    <t>1.Chọn Thuê trọ
-2.Không nhập ký tự
-3.Bấm [Lọc]</t>
-  </si>
-  <si>
     <t>Trò chuyện với admin</t>
   </si>
   <si>
@@ -514,6 +500,20 @@
   </si>
   <si>
     <t>Chưa hiển thị tên cùng đánh giá đã nhập</t>
+  </si>
+  <si>
+    <t>Tìm kiếm bằng chữ</t>
+  </si>
+  <si>
+    <t>1.Chọn Thuê trọ
+2.Nhập từ khóa vào ô tìm kiếm
+3.Bấm [Lọc]</t>
+  </si>
+  <si>
+    <t>Nhập từ khóa vào ô tìm kiếm</t>
+  </si>
+  <si>
+    <t>Không chạy tìm kiếm</t>
   </si>
 </sst>
 </file>
@@ -1231,16 +1231,16 @@
       <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="11.33203125" customWidth="1"/>
-    <col min="3" max="3" width="15.53125" customWidth="1"/>
-    <col min="4" max="4" width="34.19921875" customWidth="1"/>
-    <col min="5" max="5" width="27.1328125" customWidth="1"/>
-    <col min="6" max="6" width="15.19921875" customWidth="1"/>
+    <col min="3" max="3" width="15.5546875" customWidth="1"/>
+    <col min="4" max="4" width="34.21875" customWidth="1"/>
+    <col min="5" max="5" width="27.109375" customWidth="1"/>
+    <col min="6" max="6" width="15.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
@@ -1250,12 +1250,12 @@
       <c r="E1" s="29"/>
       <c r="F1" s="29"/>
       <c r="G1" s="28" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H1" s="28"/>
       <c r="I1" s="28"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="27" t="s">
         <v>1</v>
       </c>
@@ -1268,7 +1268,7 @@
       <c r="H2" s="27"/>
       <c r="I2" s="27"/>
     </row>
-    <row r="3" spans="1:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1288,16 +1288,16 @@
         <v>7</v>
       </c>
       <c r="G3" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="I3" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="I3" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="78.599999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    </row>
+    <row r="4" spans="1:9" ht="78.599999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="9" t="s">
         <v>8</v>
       </c>
@@ -1314,19 +1314,19 @@
         <v>12</v>
       </c>
       <c r="F4" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G4" s="13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H4" s="13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I4" s="13" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="9" t="s">
         <v>13</v>
       </c>
@@ -1341,75 +1341,75 @@
         <v>16</v>
       </c>
       <c r="F5" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G5" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H5" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I5" s="14" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="53.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="53.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B6" s="30"/>
       <c r="C6" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D6" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="F6" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="G6" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="H6" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="I6" s="14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="48.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="9" t="s">
         <v>20</v>
-      </c>
-      <c r="F6" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="G6" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="H6" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="I6" s="14" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="48.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A7" s="9" t="s">
-        <v>21</v>
       </c>
       <c r="B7" s="30"/>
       <c r="C7" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D7" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="F7" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" s="29" t="s">
         <v>23</v>
-      </c>
-      <c r="F7" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="G7" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="H7" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="I7" s="5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A10" s="29" t="s">
-        <v>24</v>
       </c>
       <c r="B10" s="29"/>
       <c r="C10" s="29"/>
@@ -1417,12 +1417,12 @@
       <c r="E10" s="29"/>
       <c r="F10" s="29"/>
       <c r="G10" s="28" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H10" s="28"/>
       <c r="I10" s="28"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="27" t="s">
         <v>1</v>
       </c>
@@ -1435,7 +1435,7 @@
       <c r="H11" s="27"/>
       <c r="I11" s="27"/>
     </row>
-    <row r="12" spans="1:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>2</v>
       </c>
@@ -1455,78 +1455,78 @@
         <v>7</v>
       </c>
       <c r="G12" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="H12" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="H12" s="2" t="s">
+      <c r="I12" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="I12" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="28.9" thickBot="1" x14ac:dyDescent="0.5">
+    </row>
+    <row r="13" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="30" t="s">
+      <c r="C13" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="D13" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="E13" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="F13" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="G13" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="H13" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="I13" s="13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="9" t="s">
         <v>29</v>
-      </c>
-      <c r="F13" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="G13" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="H13" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="I13" s="13" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="57.4" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A14" s="9" t="s">
-        <v>30</v>
       </c>
       <c r="B14" s="30"/>
       <c r="C14" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="F14" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G14" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H14" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I14" s="14" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B15" s="7"/>
       <c r="F15" s="11"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="29" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B17" s="29"/>
       <c r="C17" s="29"/>
@@ -1534,12 +1534,12 @@
       <c r="E17" s="29"/>
       <c r="F17" s="29"/>
       <c r="G17" s="28" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H17" s="28"/>
       <c r="I17" s="28"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="27" t="s">
         <v>1</v>
       </c>
@@ -1552,7 +1552,7 @@
       <c r="H18" s="27"/>
       <c r="I18" s="27"/>
     </row>
-    <row r="19" spans="1:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>2</v>
       </c>
@@ -1572,74 +1572,74 @@
         <v>7</v>
       </c>
       <c r="G19" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="H19" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="H19" s="2" t="s">
+      <c r="I19" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="I19" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="57.4" thickBot="1" x14ac:dyDescent="0.5">
+    </row>
+    <row r="20" spans="1:9" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="B20" s="26" t="s">
+      <c r="C20" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="F20" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="G20" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="H20" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="I20" s="13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="9" t="s">
         <v>33</v>
-      </c>
-      <c r="C20" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="D20" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="E20" s="10" t="s">
-        <v>86</v>
-      </c>
-      <c r="F20" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="G20" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="H20" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="I20" s="13" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" ht="57.4" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A21" s="9" t="s">
-        <v>34</v>
       </c>
       <c r="B21" s="26"/>
       <c r="C21" s="11" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D21" s="12" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E21" s="10" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="F21" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G21" s="13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H21" s="13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I21" s="13" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="29" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B24" s="29"/>
       <c r="C24" s="29"/>
@@ -1647,12 +1647,12 @@
       <c r="E24" s="29"/>
       <c r="F24" s="29"/>
       <c r="G24" s="28" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H24" s="28"/>
       <c r="I24" s="28"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="27" t="s">
         <v>1</v>
       </c>
@@ -1665,7 +1665,7 @@
       <c r="H25" s="27"/>
       <c r="I25" s="27"/>
     </row>
-    <row r="26" spans="1:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="26" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>2</v>
       </c>
@@ -1685,204 +1685,204 @@
         <v>7</v>
       </c>
       <c r="G26" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="H26" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="H26" s="2" t="s">
+      <c r="I26" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="I26" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" ht="43.15" thickBot="1" x14ac:dyDescent="0.5">
+    </row>
+    <row r="27" spans="1:9" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B27" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="B27" s="26" t="s">
+      <c r="C27" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="C27" s="8" t="s">
+      <c r="D27" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="D27" s="15" t="s">
+      <c r="E27" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="E27" s="16" t="s">
+      <c r="F27" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="F27" s="11" t="s">
+      <c r="G27" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="H27" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="I27" s="13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="9" t="s">
         <v>47</v>
-      </c>
-      <c r="G27" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="H27" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="I27" s="13" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" ht="57.4" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A28" s="9" t="s">
-        <v>48</v>
       </c>
       <c r="B28" s="26"/>
       <c r="C28" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D28" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="E28" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="E28" s="10" t="s">
+      <c r="F28" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="G28" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="H28" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="I28" s="13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="71.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="9" t="s">
         <v>50</v>
-      </c>
-      <c r="F28" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="G28" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="H28" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="I28" s="13" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" ht="71.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A29" s="9" t="s">
-        <v>51</v>
       </c>
       <c r="B29" s="26"/>
       <c r="C29" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="D29" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="D29" s="15" t="s">
+      <c r="E29" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="E29" s="12" t="s">
+      <c r="F29" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="G29" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="H29" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="I29" s="13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="9" t="s">
         <v>54</v>
-      </c>
-      <c r="F29" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="G29" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="H29" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="I29" s="13" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" ht="57.4" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A30" s="9" t="s">
-        <v>55</v>
       </c>
       <c r="B30" s="26"/>
       <c r="C30" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="D30" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="D30" s="12" t="s">
-        <v>57</v>
-      </c>
       <c r="E30" s="10" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="F30" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G30" s="13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H30" s="13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I30" s="13" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" ht="43.15" thickBot="1" x14ac:dyDescent="0.5">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="9" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B31" s="26"/>
       <c r="C31" s="8" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D31" s="15" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E31" s="10" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="F31" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G31" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H31" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I31" s="14" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" ht="57.4" thickBot="1" x14ac:dyDescent="0.5">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="9" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B32" s="26"/>
       <c r="C32" s="8" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D32" s="15" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E32" s="10" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="F32" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G32" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H32" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I32" s="14" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" ht="43.15" thickBot="1" x14ac:dyDescent="0.5">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="9" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B33" s="26"/>
       <c r="C33" s="8" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D33" s="15" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E33" s="10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F33" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G33" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H33" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I33" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -1912,25 +1912,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68FE9BBC-A729-407C-A7F1-8BCC2741D4DA}">
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12.6640625" customWidth="1"/>
-    <col min="2" max="2" width="14.53125" customWidth="1"/>
+    <col min="2" max="2" width="14.5546875" customWidth="1"/>
     <col min="3" max="3" width="12" customWidth="1"/>
-    <col min="4" max="4" width="20.19921875" customWidth="1"/>
-    <col min="5" max="5" width="15.86328125" customWidth="1"/>
-    <col min="6" max="6" width="22.53125" customWidth="1"/>
-    <col min="7" max="7" width="23.46484375" customWidth="1"/>
+    <col min="4" max="4" width="20.21875" customWidth="1"/>
+    <col min="5" max="5" width="15.88671875" customWidth="1"/>
+    <col min="6" max="6" width="22.5546875" customWidth="1"/>
+    <col min="7" max="7" width="23.44140625" customWidth="1"/>
     <col min="8" max="8" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="34" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B1" s="35"/>
       <c r="C1" s="36"/>
@@ -1942,9 +1942,9 @@
       <c r="I1" s="18"/>
       <c r="J1" s="18"/>
     </row>
-    <row r="2" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="37" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B2" s="38"/>
       <c r="C2" s="38"/>
@@ -1956,7 +1956,7 @@
       <c r="I2" s="38"/>
       <c r="J2" s="39"/>
     </row>
-    <row r="3" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="19" t="s">
         <v>2</v>
       </c>
@@ -1964,89 +1964,89 @@
         <v>3</v>
       </c>
       <c r="C3" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="D3" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="E3" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="F3" s="20" t="s">
         <v>77</v>
-      </c>
-      <c r="D3" s="21" t="s">
-        <v>78</v>
-      </c>
-      <c r="E3" s="21" t="s">
-        <v>79</v>
-      </c>
-      <c r="F3" s="20" t="s">
-        <v>80</v>
       </c>
       <c r="G3" s="20" t="s">
         <v>6</v>
       </c>
       <c r="H3" s="20" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="I3" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="J3" s="23" t="s">
         <v>61</v>
       </c>
-      <c r="J3" s="23" t="s">
+    </row>
+    <row r="4" spans="1:10" ht="70.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="B4" s="31" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" ht="70.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A4" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="B4" s="31" t="s">
+      <c r="C4" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="E4" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="F4" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="C4" s="17" t="s">
-        <v>134</v>
-      </c>
-      <c r="D4" s="17" t="s">
-        <v>132</v>
-      </c>
-      <c r="E4" s="17" t="s">
-        <v>133</v>
-      </c>
-      <c r="F4" s="17" t="s">
+      <c r="G4" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="G4" s="17" t="s">
-        <v>65</v>
-      </c>
       <c r="H4" s="17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I4" s="18"/>
       <c r="J4" s="18"/>
     </row>
-    <row r="5" spans="1:10" ht="71.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:10" ht="71.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="17" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B5" s="32"/>
       <c r="C5" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="D5" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="D5" s="17" t="s">
+      <c r="E5" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="E5" s="17" t="s">
-        <v>68</v>
-      </c>
       <c r="F5" s="17" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G5" s="17" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="H5" s="17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I5" s="18"/>
       <c r="J5" s="18"/>
     </row>
-    <row r="6" spans="1:10" ht="16.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="7" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="8" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:10" ht="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="7" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="8" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="34" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B8" s="35"/>
       <c r="C8" s="36"/>
@@ -2058,9 +2058,9 @@
       <c r="I8" s="18"/>
       <c r="J8" s="18"/>
     </row>
-    <row r="9" spans="1:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="37" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B9" s="38"/>
       <c r="C9" s="38"/>
@@ -2072,7 +2072,7 @@
       <c r="I9" s="38"/>
       <c r="J9" s="39"/>
     </row>
-    <row r="10" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="19" t="s">
         <v>2</v>
       </c>
@@ -2080,88 +2080,88 @@
         <v>3</v>
       </c>
       <c r="C10" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="D10" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="E10" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="F10" s="20" t="s">
         <v>77</v>
-      </c>
-      <c r="D10" s="21" t="s">
-        <v>78</v>
-      </c>
-      <c r="E10" s="21" t="s">
-        <v>79</v>
-      </c>
-      <c r="F10" s="20" t="s">
-        <v>80</v>
       </c>
       <c r="G10" s="20" t="s">
         <v>6</v>
       </c>
       <c r="H10" s="20" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="I10" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="J10" s="23" t="s">
         <v>61</v>
       </c>
-      <c r="J10" s="23" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="57.4" thickBot="1" x14ac:dyDescent="0.5">
+    </row>
+    <row r="11" spans="1:10" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="17" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B11" s="31" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C11" s="17" t="s">
+        <v>132</v>
+      </c>
+      <c r="D11" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="E11" s="17" t="s">
+        <v>134</v>
+      </c>
+      <c r="F11" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="D11" s="17" t="s">
-        <v>136</v>
-      </c>
-      <c r="E11" s="17" t="s">
-        <v>137</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>138</v>
-      </c>
       <c r="G11" s="17" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H11" s="17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I11" s="18"/>
       <c r="J11" s="18"/>
     </row>
-    <row r="12" spans="1:10" ht="43.15" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:10" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="17" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B12" s="33"/>
       <c r="C12" s="17" t="s">
-        <v>72</v>
+        <v>142</v>
       </c>
       <c r="D12" s="17" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="E12" s="17" t="s">
-        <v>17</v>
+        <v>144</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G12" s="17" t="s">
-        <v>71</v>
+        <v>145</v>
       </c>
       <c r="H12" s="17" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="I12" s="18"/>
       <c r="J12" s="18"/>
     </row>
-    <row r="13" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="14" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="14" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="34" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B14" s="35"/>
       <c r="C14" s="36"/>
@@ -2173,9 +2173,9 @@
       <c r="I14" s="18"/>
       <c r="J14" s="18"/>
     </row>
-    <row r="15" spans="1:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="37" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B15" s="38"/>
       <c r="C15" s="38"/>
@@ -2187,7 +2187,7 @@
       <c r="I15" s="38"/>
       <c r="J15" s="39"/>
     </row>
-    <row r="16" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="19" t="s">
         <v>2</v>
       </c>
@@ -2195,88 +2195,88 @@
         <v>3</v>
       </c>
       <c r="C16" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="D16" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="E16" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="F16" s="20" t="s">
         <v>77</v>
-      </c>
-      <c r="D16" s="21" t="s">
-        <v>78</v>
-      </c>
-      <c r="E16" s="21" t="s">
-        <v>79</v>
-      </c>
-      <c r="F16" s="20" t="s">
-        <v>80</v>
       </c>
       <c r="G16" s="20" t="s">
         <v>6</v>
       </c>
       <c r="H16" s="20" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="I16" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="J16" s="23" t="s">
         <v>61</v>
       </c>
-      <c r="J16" s="23" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="71.650000000000006" thickBot="1" x14ac:dyDescent="0.5">
+    </row>
+    <row r="17" spans="1:10" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="24" t="s">
+        <v>100</v>
+      </c>
+      <c r="B17" s="31" t="s">
+        <v>105</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="D17" s="17" t="s">
+        <v>137</v>
+      </c>
+      <c r="E17" s="24" t="s">
+        <v>102</v>
+      </c>
+      <c r="F17" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="B17" s="31" t="s">
-        <v>108</v>
-      </c>
-      <c r="C17" s="12" t="s">
-        <v>104</v>
-      </c>
-      <c r="D17" s="17" t="s">
-        <v>141</v>
-      </c>
-      <c r="E17" s="24" t="s">
-        <v>105</v>
-      </c>
-      <c r="F17" s="8" t="s">
-        <v>106</v>
-      </c>
       <c r="G17" s="8" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="H17" s="17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I17" s="18"/>
       <c r="J17" s="18"/>
     </row>
-    <row r="18" spans="1:10" ht="43.15" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:10" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="17" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B18" s="33"/>
       <c r="C18" s="17" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="D18" s="17" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="E18" s="17" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="G18" s="8" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="H18" s="17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I18" s="18"/>
       <c r="J18" s="18"/>
     </row>
-    <row r="20" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="21" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="21" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="34" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B21" s="35"/>
       <c r="C21" s="36"/>
@@ -2288,9 +2288,9 @@
       <c r="I21" s="18"/>
       <c r="J21" s="18"/>
     </row>
-    <row r="22" spans="1:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="37" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B22" s="38"/>
       <c r="C22" s="38"/>
@@ -2302,7 +2302,7 @@
       <c r="I22" s="38"/>
       <c r="J22" s="39"/>
     </row>
-    <row r="23" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="19" t="s">
         <v>2</v>
       </c>
@@ -2310,132 +2310,132 @@
         <v>3</v>
       </c>
       <c r="C23" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="D23" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="E23" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="F23" s="20" t="s">
         <v>77</v>
-      </c>
-      <c r="D23" s="21" t="s">
-        <v>78</v>
-      </c>
-      <c r="E23" s="21" t="s">
-        <v>79</v>
-      </c>
-      <c r="F23" s="20" t="s">
-        <v>80</v>
       </c>
       <c r="G23" s="20" t="s">
         <v>6</v>
       </c>
       <c r="H23" s="20" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="I23" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="J23" s="23" t="s">
         <v>61</v>
       </c>
-      <c r="J23" s="23" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" ht="57.4" thickBot="1" x14ac:dyDescent="0.5">
+    </row>
+    <row r="24" spans="1:10" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="24" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B24" s="31" t="s">
+        <v>107</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="D24" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="E24" s="25" t="s">
         <v>110</v>
       </c>
-      <c r="C24" s="12" t="s">
+      <c r="F24" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="D24" s="17" t="s">
-        <v>112</v>
-      </c>
-      <c r="E24" s="25" t="s">
-        <v>113</v>
-      </c>
-      <c r="F24" s="8" t="s">
-        <v>114</v>
-      </c>
       <c r="G24" s="8" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="H24" s="17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I24" s="18"/>
       <c r="J24" s="18"/>
     </row>
-    <row r="25" spans="1:10" ht="57.4" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="25" spans="1:10" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="17" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B25" s="32"/>
       <c r="C25" s="17" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D25" s="17" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="E25" s="17" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="H25" s="17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I25" s="18"/>
       <c r="J25" s="18"/>
     </row>
-    <row r="26" spans="1:10" ht="43.15" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="26" spans="1:10" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="17" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B26" s="32"/>
       <c r="C26" s="17" t="s">
+        <v>118</v>
+      </c>
+      <c r="D26" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="E26" s="17" t="s">
         <v>121</v>
       </c>
-      <c r="D26" s="17" t="s">
+      <c r="F26" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="E26" s="17" t="s">
-        <v>124</v>
-      </c>
-      <c r="F26" s="5" t="s">
-        <v>125</v>
-      </c>
       <c r="G26" s="5" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="H26" s="17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I26" s="18"/>
       <c r="J26" s="18"/>
     </row>
-    <row r="27" spans="1:10" ht="28.9" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="27" spans="1:10" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="17" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="B27" s="33"/>
       <c r="C27" s="17" t="s">
+        <v>123</v>
+      </c>
+      <c r="D27" s="17" t="s">
+        <v>124</v>
+      </c>
+      <c r="E27" s="17" t="s">
+        <v>125</v>
+      </c>
+      <c r="F27" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="D27" s="17" t="s">
-        <v>127</v>
-      </c>
-      <c r="E27" s="17" t="s">
-        <v>128</v>
-      </c>
-      <c r="F27" s="5" t="s">
-        <v>129</v>
-      </c>
       <c r="G27" s="5" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="H27" s="17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I27" s="18"/>
       <c r="J27" s="18"/>

</xml_diff>

<commit_message>
Kiểm thử lần cuối của MHIEU
</commit_message>
<xml_diff>
--- a/Sprint 2/Tài liệu đặc tả yêu cầu/Kiểm thử ONLY QUẠT PART 2.xlsx
+++ b/Sprint 2/Tài liệu đặc tả yêu cầu/Kiểm thử ONLY QUẠT PART 2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Acer\Documents\GitHub\BCS\Sprint 2\Tài liệu đặc tả yêu cầu\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://wru-my.sharepoint.com/personal/2251061780_e_tlu_edu_vn/Documents/Tài liệu/GitHub/BCS/Sprint 2/Tài liệu đặc tả yêu cầu/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{671256D1-55DC-4DE3-B9A5-E171AC26DD9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{671256D1-55DC-4DE3-B9A5-E171AC26DD9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6E34D1AF-49F0-4F28-9191-165AB0AA2E6B}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{C21961AB-009A-468A-8C50-42DFE010BB31}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="1" xr2:uid="{C21961AB-009A-468A-8C50-42DFE010BB31}"/>
   </bookViews>
   <sheets>
     <sheet name="Giao diện" sheetId="1" r:id="rId1"/>
@@ -436,10 +436,6 @@
     <t>Lưu bài viết</t>
   </si>
   <si>
-    <t>1.Xem bài viết
-2.Nhấn [Lưu lại]</t>
-  </si>
-  <si>
     <t>Lưu thử 1 bài bất kì</t>
   </si>
   <si>
@@ -484,15 +480,6 @@
     <t>Trò chuyện với admin</t>
   </si>
   <si>
-    <t xml:space="preserve">1.Nhấn bài viết
-2.Chọn [Liên hệ]    3.Nhập chữ hoặc số vào khung chat
-</t>
-  </si>
-  <si>
-    <t>1.Chọn [Chat với admin]
-2.Nhập chữ hoặc số vào khung chat</t>
-  </si>
-  <si>
     <t>Hiện thị tên cùng đánh giá đã nhập</t>
   </si>
   <si>
@@ -514,6 +501,19 @@
   </si>
   <si>
     <t>Không chạy tìm kiếm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.Nhấn bài viết
+2.Chọn [Chat với chủ trọ]          3.Nhập chữ hoặc số vào khung chat                     4.Gửi đi
+</t>
+  </si>
+  <si>
+    <t>1.Chọn [Chat với admin]
+2.Nhập chữ hoặc số vào khung chat                    3.Gửi đi</t>
+  </si>
+  <si>
+    <t>1.Xem bài viết
+2.Nhấn [Lưu bài]</t>
   </si>
 </sst>
 </file>
@@ -1231,16 +1231,16 @@
       <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="2" max="2" width="11.33203125" customWidth="1"/>
-    <col min="3" max="3" width="15.5546875" customWidth="1"/>
-    <col min="4" max="4" width="34.21875" customWidth="1"/>
-    <col min="5" max="5" width="27.109375" customWidth="1"/>
-    <col min="6" max="6" width="15.21875" customWidth="1"/>
+    <col min="3" max="3" width="15.53125" customWidth="1"/>
+    <col min="4" max="4" width="34.19921875" customWidth="1"/>
+    <col min="5" max="5" width="27.1328125" customWidth="1"/>
+    <col min="6" max="6" width="15.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
@@ -1255,7 +1255,7 @@
       <c r="H1" s="28"/>
       <c r="I1" s="28"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A2" s="27" t="s">
         <v>1</v>
       </c>
@@ -1268,7 +1268,7 @@
       <c r="H2" s="27"/>
       <c r="I2" s="27"/>
     </row>
-    <row r="3" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1297,7 +1297,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="78.599999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" ht="78.599999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A4" s="9" t="s">
         <v>8</v>
       </c>
@@ -1326,7 +1326,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A5" s="9" t="s">
         <v>13</v>
       </c>
@@ -1353,7 +1353,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="53.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" ht="53.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A6" s="9" t="s">
         <v>17</v>
       </c>
@@ -1380,7 +1380,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="48.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" ht="48.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A7" s="9" t="s">
         <v>20</v>
       </c>
@@ -1407,7 +1407,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A10" s="29" t="s">
         <v>23</v>
       </c>
@@ -1422,7 +1422,7 @@
       <c r="H10" s="28"/>
       <c r="I10" s="28"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A11" s="27" t="s">
         <v>1</v>
       </c>
@@ -1435,7 +1435,7 @@
       <c r="H11" s="27"/>
       <c r="I11" s="27"/>
     </row>
-    <row r="12" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A12" s="1" t="s">
         <v>2</v>
       </c>
@@ -1464,7 +1464,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" ht="28.9" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A13" s="9" t="s">
         <v>24</v>
       </c>
@@ -1493,7 +1493,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" ht="57.4" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A14" s="9" t="s">
         <v>29</v>
       </c>
@@ -1502,10 +1502,10 @@
         <v>30</v>
       </c>
       <c r="D14" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="E14" s="6" t="s">
         <v>127</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>128</v>
       </c>
       <c r="F14" s="11" t="s">
         <v>46</v>
@@ -1520,11 +1520,11 @@
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
       <c r="B15" s="7"/>
       <c r="F15" s="11"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A17" s="29" t="s">
         <v>79</v>
       </c>
@@ -1539,7 +1539,7 @@
       <c r="H17" s="28"/>
       <c r="I17" s="28"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A18" s="27" t="s">
         <v>1</v>
       </c>
@@ -1552,7 +1552,7 @@
       <c r="H18" s="27"/>
       <c r="I18" s="27"/>
     </row>
-    <row r="19" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A19" s="1" t="s">
         <v>2</v>
       </c>
@@ -1581,7 +1581,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" ht="57.4" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A20" s="9" t="s">
         <v>31</v>
       </c>
@@ -1610,7 +1610,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" ht="57.4" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A21" s="9" t="s">
         <v>33</v>
       </c>
@@ -1637,7 +1637,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A24" s="29" t="s">
         <v>40</v>
       </c>
@@ -1652,7 +1652,7 @@
       <c r="H24" s="28"/>
       <c r="I24" s="28"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A25" s="27" t="s">
         <v>1</v>
       </c>
@@ -1665,7 +1665,7 @@
       <c r="H25" s="27"/>
       <c r="I25" s="27"/>
     </row>
-    <row r="26" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A26" s="1" t="s">
         <v>2</v>
       </c>
@@ -1694,7 +1694,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:9" ht="43.15" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A27" s="9" t="s">
         <v>41</v>
       </c>
@@ -1723,7 +1723,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:9" ht="57.4" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A28" s="9" t="s">
         <v>47</v>
       </c>
@@ -1750,7 +1750,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="71.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:9" ht="71.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A29" s="9" t="s">
         <v>50</v>
       </c>
@@ -1777,7 +1777,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:9" ht="57.4" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A30" s="9" t="s">
         <v>54</v>
       </c>
@@ -1804,7 +1804,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:9" ht="43.15" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A31" s="9" t="s">
         <v>86</v>
       </c>
@@ -1831,7 +1831,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:9" ht="57.4" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A32" s="9" t="s">
         <v>98</v>
       </c>
@@ -1858,7 +1858,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="33" spans="1:9" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:9" ht="43.15" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A33" s="9" t="s">
         <v>99</v>
       </c>
@@ -1912,23 +1912,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68FE9BBC-A729-407C-A7F1-8BCC2741D4DA}">
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="L28" sqref="L28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="12.6640625" customWidth="1"/>
-    <col min="2" max="2" width="14.5546875" customWidth="1"/>
+    <col min="2" max="2" width="14.53125" customWidth="1"/>
     <col min="3" max="3" width="12" customWidth="1"/>
-    <col min="4" max="4" width="20.21875" customWidth="1"/>
-    <col min="5" max="5" width="15.88671875" customWidth="1"/>
-    <col min="6" max="6" width="22.5546875" customWidth="1"/>
-    <col min="7" max="7" width="23.44140625" customWidth="1"/>
+    <col min="4" max="4" width="22.265625" customWidth="1"/>
+    <col min="5" max="5" width="15.86328125" customWidth="1"/>
+    <col min="6" max="6" width="22.53125" customWidth="1"/>
+    <col min="7" max="7" width="23.46484375" customWidth="1"/>
     <col min="8" max="8" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A1" s="34" t="s">
         <v>58</v>
       </c>
@@ -1942,7 +1942,7 @@
       <c r="I1" s="18"/>
       <c r="J1" s="18"/>
     </row>
-    <row r="2" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A2" s="37" t="s">
         <v>59</v>
       </c>
@@ -1956,7 +1956,7 @@
       <c r="I2" s="38"/>
       <c r="J2" s="39"/>
     </row>
-    <row r="3" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A3" s="19" t="s">
         <v>2</v>
       </c>
@@ -1988,7 +1988,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="70.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" ht="70.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A4" s="17" t="s">
         <v>70</v>
       </c>
@@ -1996,13 +1996,13 @@
         <v>62</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D4" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="E4" s="17" t="s">
         <v>129</v>
-      </c>
-      <c r="E4" s="17" t="s">
-        <v>130</v>
       </c>
       <c r="F4" s="17" t="s">
         <v>63</v>
@@ -2016,7 +2016,7 @@
       <c r="I4" s="18"/>
       <c r="J4" s="18"/>
     </row>
-    <row r="5" spans="1:10" ht="71.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" ht="71.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A5" s="17" t="s">
         <v>71</v>
       </c>
@@ -2031,10 +2031,10 @@
         <v>67</v>
       </c>
       <c r="F5" s="17" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="G5" s="17" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="H5" s="17" t="s">
         <v>38</v>
@@ -2042,9 +2042,9 @@
       <c r="I5" s="18"/>
       <c r="J5" s="18"/>
     </row>
-    <row r="6" spans="1:10" ht="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="7" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="8" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" ht="16.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="7" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="8" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A8" s="34" t="s">
         <v>96</v>
       </c>
@@ -2058,7 +2058,7 @@
       <c r="I8" s="18"/>
       <c r="J8" s="18"/>
     </row>
-    <row r="9" spans="1:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A9" s="37" t="s">
         <v>59</v>
       </c>
@@ -2072,7 +2072,7 @@
       <c r="I9" s="38"/>
       <c r="J9" s="39"/>
     </row>
-    <row r="10" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A10" s="19" t="s">
         <v>2</v>
       </c>
@@ -2104,7 +2104,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" ht="57.4" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A11" s="17" t="s">
         <v>72</v>
       </c>
@@ -2112,16 +2112,16 @@
         <v>68</v>
       </c>
       <c r="C11" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="D11" s="17" t="s">
         <v>132</v>
       </c>
-      <c r="D11" s="17" t="s">
+      <c r="E11" s="17" t="s">
         <v>133</v>
       </c>
-      <c r="E11" s="17" t="s">
+      <c r="F11" s="5" t="s">
         <v>134</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>135</v>
       </c>
       <c r="G11" s="17" t="s">
         <v>64</v>
@@ -2132,25 +2132,25 @@
       <c r="I11" s="18"/>
       <c r="J11" s="18"/>
     </row>
-    <row r="12" spans="1:10" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" ht="57.4" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A12" s="17" t="s">
         <v>73</v>
       </c>
       <c r="B12" s="33"/>
       <c r="C12" s="17" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="D12" s="17" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="E12" s="17" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="F12" s="5" t="s">
         <v>69</v>
       </c>
       <c r="G12" s="17" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="H12" s="17" t="s">
         <v>38</v>
@@ -2158,8 +2158,8 @@
       <c r="I12" s="18"/>
       <c r="J12" s="18"/>
     </row>
-    <row r="13" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="14" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="14" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A14" s="34" t="s">
         <v>97</v>
       </c>
@@ -2173,7 +2173,7 @@
       <c r="I14" s="18"/>
       <c r="J14" s="18"/>
     </row>
-    <row r="15" spans="1:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A15" s="37" t="s">
         <v>59</v>
       </c>
@@ -2187,7 +2187,7 @@
       <c r="I15" s="38"/>
       <c r="J15" s="39"/>
     </row>
-    <row r="16" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A16" s="19" t="s">
         <v>2</v>
       </c>
@@ -2219,7 +2219,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" ht="85.9" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A17" s="24" t="s">
         <v>100</v>
       </c>
@@ -2230,7 +2230,7 @@
         <v>101</v>
       </c>
       <c r="D17" s="17" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="E17" s="24" t="s">
         <v>102</v>
@@ -2247,16 +2247,16 @@
       <c r="I17" s="18"/>
       <c r="J17" s="18"/>
     </row>
-    <row r="18" spans="1:10" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" ht="57.4" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A18" s="17" t="s">
         <v>104</v>
       </c>
       <c r="B18" s="33"/>
       <c r="C18" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D18" s="17" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="E18" s="17" t="s">
         <v>102</v>
@@ -2273,8 +2273,8 @@
       <c r="I18" s="18"/>
       <c r="J18" s="18"/>
     </row>
-    <row r="20" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="21" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="21" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A21" s="34" t="s">
         <v>106</v>
       </c>
@@ -2288,7 +2288,7 @@
       <c r="I21" s="18"/>
       <c r="J21" s="18"/>
     </row>
-    <row r="22" spans="1:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A22" s="37" t="s">
         <v>59</v>
       </c>
@@ -2302,7 +2302,7 @@
       <c r="I22" s="38"/>
       <c r="J22" s="39"/>
     </row>
-    <row r="23" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A23" s="19" t="s">
         <v>2</v>
       </c>
@@ -2334,7 +2334,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:10" ht="57.4" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A24" s="24" t="s">
         <v>112</v>
       </c>
@@ -2362,7 +2362,7 @@
       <c r="I24" s="18"/>
       <c r="J24" s="18"/>
     </row>
-    <row r="25" spans="1:10" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:10" ht="57.4" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A25" s="17" t="s">
         <v>113</v>
       </c>
@@ -2388,7 +2388,7 @@
       <c r="I25" s="18"/>
       <c r="J25" s="18"/>
     </row>
-    <row r="26" spans="1:10" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:10" ht="43.15" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A26" s="17" t="s">
         <v>117</v>
       </c>
@@ -2414,25 +2414,25 @@
       <c r="I26" s="18"/>
       <c r="J26" s="18"/>
     </row>
-    <row r="27" spans="1:10" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:10" ht="28.9" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A27" s="17" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B27" s="33"/>
       <c r="C27" s="17" t="s">
         <v>123</v>
       </c>
       <c r="D27" s="17" t="s">
+        <v>145</v>
+      </c>
+      <c r="E27" s="17" t="s">
         <v>124</v>
       </c>
-      <c r="E27" s="17" t="s">
+      <c r="F27" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="F27" s="5" t="s">
-        <v>126</v>
-      </c>
       <c r="G27" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H27" s="17" t="s">
         <v>39</v>

</xml_diff>